<commit_message>
Updates to U18Image processing  and ML_EO
</commit_message>
<xml_diff>
--- a/Photos/U18/Imagenes_raw_preformato.xlsx
+++ b/Photos/U18/Imagenes_raw_preformato.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/PycharmProjects/CoreImages/Photos/U18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4806F19B-35F6-544E-8EDB-D4E6D9AEF84B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7192E8E2-9A3D-FF46-A6AD-DD7CF4CD08F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="2940" windowWidth="29440" windowHeight="15700" xr2:uid="{39C79890-D145-4807-8F9E-7D03B26FE3B0}"/>
+    <workbookView xWindow="16300" yWindow="2900" windowWidth="30100" windowHeight="16440" xr2:uid="{39C79890-D145-4807-8F9E-7D03B26FE3B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +153,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB700CD"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,43 +311,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -349,6 +374,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB700CD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1099,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46D7737-5E7A-4AB0-B8E1-D0EC24ABA82F}">
   <dimension ref="B1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1149,16 +1179,16 @@
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J3" s="23">
+      <c r="J3" s="25">
         <v>1</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="33">
         <v>710</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="25">
         <f>J45+1</f>
         <v>9</v>
       </c>
@@ -1168,7 +1198,7 @@
       <c r="P3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="23">
+      <c r="R3" s="25">
         <f>N45+1</f>
         <v>17</v>
       </c>
@@ -1180,23 +1210,23 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J4" s="24"/>
-      <c r="K4" s="5">
+      <c r="J4" s="26"/>
+      <c r="K4" s="34">
         <v>712.95</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="N4" s="24"/>
+      <c r="L4" s="23"/>
+      <c r="N4" s="26"/>
       <c r="O4" s="5">
         <v>835.95</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="24"/>
+      <c r="R4" s="26"/>
       <c r="S4" s="5">
         <v>957</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1209,21 +1239,21 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="5">
+      <c r="J5" s="26"/>
+      <c r="K5" s="34">
         <v>715.95</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="N5" s="24"/>
+      <c r="L5" s="23"/>
+      <c r="N5" s="26"/>
       <c r="O5" s="5">
         <v>838.9</v>
       </c>
-      <c r="P5" s="21"/>
-      <c r="R5" s="24"/>
+      <c r="P5" s="23"/>
+      <c r="R5" s="26"/>
       <c r="S5" s="5">
         <v>960</v>
       </c>
-      <c r="T5" s="21"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="19"/>
@@ -1234,21 +1264,21 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="5">
+      <c r="J6" s="26"/>
+      <c r="K6" s="34">
         <v>718.95</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="N6" s="24"/>
+      <c r="L6" s="23"/>
+      <c r="N6" s="26"/>
       <c r="O6" s="5">
         <v>841.9</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="R6" s="24"/>
+      <c r="P6" s="23"/>
+      <c r="R6" s="26"/>
       <c r="S6" s="5">
         <v>963</v>
       </c>
-      <c r="T6" s="21"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" s="19"/>
@@ -1259,21 +1289,21 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="5">
+      <c r="J7" s="26"/>
+      <c r="K7" s="34">
         <v>721.95</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="N7" s="24"/>
+      <c r="L7" s="23"/>
+      <c r="N7" s="26"/>
       <c r="O7" s="5">
         <v>844.9</v>
       </c>
-      <c r="P7" s="21"/>
-      <c r="R7" s="24"/>
+      <c r="P7" s="23"/>
+      <c r="R7" s="26"/>
       <c r="S7" s="5">
         <v>965.9</v>
       </c>
-      <c r="T7" s="21"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
@@ -1284,21 +1314,21 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="6">
+      <c r="J8" s="27"/>
+      <c r="K8" s="35">
         <v>724.95</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="N8" s="25"/>
+      <c r="L8" s="28"/>
+      <c r="N8" s="27"/>
       <c r="O8" s="6">
         <v>847.95</v>
       </c>
-      <c r="P8" s="22"/>
-      <c r="R8" s="25"/>
+      <c r="P8" s="28"/>
+      <c r="R8" s="27"/>
       <c r="S8" s="6">
         <v>968.95</v>
       </c>
-      <c r="T8" s="22"/>
+      <c r="T8" s="28"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="19"/>
@@ -1309,33 +1339,33 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="23">
+      <c r="J9" s="25">
         <v>2</v>
       </c>
       <c r="K9" s="4">
         <v>727.95</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="25">
         <f>N3+1</f>
         <v>10</v>
       </c>
       <c r="O9" s="4">
         <v>850.95</v>
       </c>
-      <c r="P9" s="20" t="s">
+      <c r="P9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="25">
         <f>R3+1</f>
         <v>18</v>
       </c>
       <c r="S9" s="4">
         <v>972</v>
       </c>
-      <c r="T9" s="20" t="s">
+      <c r="T9" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1348,21 +1378,21 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="24"/>
+      <c r="J10" s="26"/>
       <c r="K10" s="5">
         <v>730.95</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="N10" s="24"/>
+      <c r="L10" s="23"/>
+      <c r="N10" s="26"/>
       <c r="O10" s="5">
         <v>853.95</v>
       </c>
-      <c r="P10" s="21"/>
-      <c r="R10" s="24"/>
+      <c r="P10" s="23"/>
+      <c r="R10" s="26"/>
       <c r="S10" s="5">
         <v>975</v>
       </c>
-      <c r="T10" s="21"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="19"/>
@@ -1373,17 +1403,17 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="5">
         <v>733.9</v>
       </c>
-      <c r="L11" s="21"/>
-      <c r="N11" s="24"/>
+      <c r="L11" s="23"/>
+      <c r="N11" s="26"/>
       <c r="O11" s="5">
         <v>856.9</v>
       </c>
-      <c r="P11" s="21"/>
-      <c r="R11" s="24"/>
+      <c r="P11" s="23"/>
+      <c r="R11" s="26"/>
       <c r="S11" s="5">
         <v>978</v>
       </c>
@@ -1400,21 +1430,21 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="24"/>
+      <c r="J12" s="26"/>
       <c r="K12" s="5">
         <v>736.9</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="24"/>
+      <c r="N12" s="26"/>
       <c r="O12" s="5">
         <v>859.9</v>
       </c>
       <c r="P12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="24"/>
+      <c r="R12" s="26"/>
       <c r="S12" s="5">
         <v>980</v>
       </c>
@@ -1431,21 +1461,21 @@
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="24"/>
+      <c r="J13" s="26"/>
       <c r="K13" s="5">
         <v>738.95</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="24"/>
+      <c r="N13" s="26"/>
       <c r="O13" s="5">
         <v>861.6</v>
       </c>
       <c r="P13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="24"/>
+      <c r="R13" s="26"/>
       <c r="S13" s="5">
         <v>981.95</v>
       </c>
@@ -1462,21 +1492,21 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="25"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="6">
         <v>739.25</v>
       </c>
       <c r="L14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="27"/>
       <c r="O14" s="6">
         <v>862.9</v>
       </c>
       <c r="P14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R14" s="25"/>
+      <c r="R14" s="27"/>
       <c r="S14" s="6">
         <v>983.65</v>
       </c>
@@ -1493,33 +1523,33 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="23">
+      <c r="J15" s="25">
         <v>3</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="36">
         <v>741.9</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="L15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="25">
         <f t="shared" ref="N15" si="0">N9+1</f>
         <v>11</v>
       </c>
-      <c r="O15" s="30">
+      <c r="O15" s="20">
         <v>864.75</v>
       </c>
-      <c r="P15" s="20" t="s">
+      <c r="P15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="25">
         <f t="shared" ref="R15" si="1">R9+1</f>
         <v>19</v>
       </c>
-      <c r="S15" s="9">
+      <c r="S15" s="36">
         <v>986.2</v>
       </c>
-      <c r="T15" s="20" t="s">
+      <c r="T15" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1532,22 +1562,22 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="10">
+      <c r="J16" s="26"/>
+      <c r="K16" s="37">
         <v>744.9</v>
       </c>
-      <c r="L16" s="21"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="31">
+      <c r="L16" s="23"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="21">
         <f>O15+3</f>
         <v>867.75</v>
       </c>
-      <c r="P16" s="21"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="10">
+      <c r="P16" s="23"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="37">
         <v>989</v>
       </c>
-      <c r="T16" s="21"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B17" s="19"/>
@@ -1558,22 +1588,22 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="10">
+      <c r="J17" s="26"/>
+      <c r="K17" s="37">
         <v>747.9</v>
       </c>
-      <c r="L17" s="21"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="31">
+      <c r="L17" s="23"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="21">
         <f t="shared" ref="O17:O20" si="2">O16+3</f>
         <v>870.75</v>
       </c>
-      <c r="P17" s="21"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="10">
+      <c r="P17" s="23"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="37">
         <v>992.2</v>
       </c>
-      <c r="T17" s="21"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
@@ -1584,23 +1614,23 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="10">
+      <c r="J18" s="26"/>
+      <c r="K18" s="37">
         <f>K17+3</f>
         <v>750.9</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="31">
+      <c r="L18" s="23"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="21">
         <f t="shared" si="2"/>
         <v>873.75</v>
       </c>
-      <c r="P18" s="21"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="10">
+      <c r="P18" s="23"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="37">
         <v>995.15</v>
       </c>
-      <c r="T18" s="21"/>
+      <c r="T18" s="23"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
@@ -1611,23 +1641,23 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="10">
+      <c r="J19" s="26"/>
+      <c r="K19" s="37">
         <f t="shared" ref="K19:K20" si="3">K18+3</f>
         <v>753.9</v>
       </c>
-      <c r="L19" s="21"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="31">
+      <c r="L19" s="23"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="21">
         <f t="shared" si="2"/>
         <v>876.75</v>
       </c>
-      <c r="P19" s="21"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="10">
+      <c r="P19" s="23"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="37">
         <v>998.15</v>
       </c>
-      <c r="T19" s="21"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="20" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
@@ -1638,23 +1668,23 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="11">
+      <c r="J20" s="27"/>
+      <c r="K20" s="38">
         <f t="shared" si="3"/>
         <v>756.9</v>
       </c>
-      <c r="L20" s="22"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="31">
+      <c r="L20" s="28"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="21">
         <f t="shared" si="2"/>
         <v>879.75</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="10">
+      <c r="P20" s="28"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="37">
         <v>1001.1</v>
       </c>
-      <c r="T20" s="22"/>
+      <c r="T20" s="28"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
@@ -1665,16 +1695,16 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
-      <c r="J21" s="23">
+      <c r="J21" s="25">
         <v>4</v>
       </c>
       <c r="K21" s="9">
         <v>759.95</v>
       </c>
-      <c r="L21" s="20" t="s">
+      <c r="L21" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="25">
         <f t="shared" ref="N21" si="4">N15+1</f>
         <v>12</v>
       </c>
@@ -1682,17 +1712,17 @@
         <f>O20+3</f>
         <v>882.75</v>
       </c>
-      <c r="P21" s="20" t="s">
+      <c r="P21" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="25">
         <f t="shared" ref="R21" si="5">R15+1</f>
         <v>20</v>
       </c>
       <c r="S21" s="9">
         <v>1004.1</v>
       </c>
-      <c r="T21" s="20" t="s">
+      <c r="T21" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1705,22 +1735,22 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
-      <c r="J22" s="24"/>
+      <c r="J22" s="26"/>
       <c r="K22" s="10">
         <v>763</v>
       </c>
-      <c r="L22" s="21"/>
-      <c r="N22" s="24"/>
+      <c r="L22" s="23"/>
+      <c r="N22" s="26"/>
       <c r="O22" s="10">
         <f>O21+3</f>
         <v>885.75</v>
       </c>
-      <c r="P22" s="21"/>
-      <c r="R22" s="24"/>
+      <c r="P22" s="23"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="10">
         <v>1007.1</v>
       </c>
-      <c r="T22" s="21"/>
+      <c r="T22" s="23"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
@@ -1731,26 +1761,26 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="26"/>
       <c r="K23" s="14">
         <v>766.1</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N23" s="24"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="10">
         <f t="shared" ref="O23" si="6">O22+3</f>
         <v>888.75</v>
       </c>
-      <c r="P23" s="26" t="s">
+      <c r="P23" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="R23" s="24"/>
+      <c r="R23" s="26"/>
       <c r="S23" s="10">
         <v>1010.1</v>
       </c>
-      <c r="T23" s="21"/>
+      <c r="T23" s="23"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B24" s="19"/>
@@ -1761,19 +1791,19 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
-      <c r="J24" s="24"/>
+      <c r="J24" s="26"/>
       <c r="K24" s="10">
         <v>768.1</v>
       </c>
-      <c r="L24" s="21" t="s">
+      <c r="L24" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="N24" s="24"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="10">
         <v>890.75</v>
       </c>
-      <c r="P24" s="26"/>
-      <c r="R24" s="24"/>
+      <c r="P24" s="32"/>
+      <c r="R24" s="26"/>
       <c r="S24" s="10">
         <v>1013.1</v>
       </c>
@@ -1790,19 +1820,19 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
-      <c r="J25" s="24"/>
+      <c r="J25" s="26"/>
       <c r="K25" s="10">
         <v>769.55</v>
       </c>
-      <c r="L25" s="21"/>
-      <c r="N25" s="24"/>
+      <c r="L25" s="23"/>
+      <c r="N25" s="26"/>
       <c r="O25" s="10">
         <v>892.75</v>
       </c>
       <c r="P25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="R25" s="24"/>
+      <c r="R25" s="26"/>
       <c r="S25" s="10" t="s">
         <v>8</v>
       </c>
@@ -1811,21 +1841,21 @@
       </c>
     </row>
     <row r="26" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="25"/>
+      <c r="J26" s="27"/>
       <c r="K26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="L26" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N26" s="25"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="P26" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="R26" s="25"/>
+      <c r="R26" s="27"/>
       <c r="S26" s="11" t="s">
         <v>8</v>
       </c>
@@ -1834,17 +1864,17 @@
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J27" s="23">
+      <c r="J27" s="25">
         <f>J21+1</f>
         <v>5</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="33">
         <v>771</v>
       </c>
-      <c r="L27" s="20" t="s">
+      <c r="L27" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N27" s="23">
+      <c r="N27" s="25">
         <f t="shared" ref="N27" si="7">N21+1</f>
         <v>13</v>
       </c>
@@ -1856,12 +1886,12 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J28" s="24"/>
-      <c r="K28" s="5">
+      <c r="J28" s="26"/>
+      <c r="K28" s="34">
         <v>774.1</v>
       </c>
-      <c r="L28" s="21"/>
-      <c r="N28" s="24"/>
+      <c r="L28" s="23"/>
+      <c r="N28" s="26"/>
       <c r="O28" s="5">
         <v>897</v>
       </c>
@@ -1870,59 +1900,59 @@
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J29" s="24"/>
-      <c r="K29" s="5">
+      <c r="J29" s="26"/>
+      <c r="K29" s="34">
         <v>777.15</v>
       </c>
-      <c r="L29" s="21"/>
-      <c r="N29" s="24"/>
+      <c r="L29" s="23"/>
+      <c r="N29" s="26"/>
       <c r="O29" s="5">
         <v>899.95</v>
       </c>
-      <c r="P29" s="21" t="s">
+      <c r="P29" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J30" s="24"/>
-      <c r="K30" s="5">
+      <c r="J30" s="26"/>
+      <c r="K30" s="34">
         <v>780.1</v>
       </c>
-      <c r="L30" s="21"/>
-      <c r="N30" s="24"/>
+      <c r="L30" s="23"/>
+      <c r="N30" s="26"/>
       <c r="O30" s="5">
         <v>902.95</v>
       </c>
-      <c r="P30" s="21"/>
+      <c r="P30" s="23"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J31" s="24"/>
-      <c r="K31" s="5">
+      <c r="J31" s="26"/>
+      <c r="K31" s="34">
         <v>783.05</v>
       </c>
-      <c r="L31" s="21"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="23"/>
+      <c r="N31" s="26"/>
       <c r="O31" s="5">
         <f>O30+3</f>
         <v>905.95</v>
       </c>
-      <c r="P31" s="21"/>
+      <c r="P31" s="23"/>
     </row>
     <row r="32" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="25"/>
-      <c r="K32" s="6">
+      <c r="J32" s="27"/>
+      <c r="K32" s="35">
         <v>786.05</v>
       </c>
-      <c r="L32" s="22"/>
-      <c r="N32" s="25"/>
+      <c r="L32" s="28"/>
+      <c r="N32" s="27"/>
       <c r="O32" s="6">
         <f>O31+3</f>
         <v>908.95</v>
       </c>
-      <c r="P32" s="22"/>
+      <c r="P32" s="28"/>
     </row>
     <row r="33" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J33" s="23">
+      <c r="J33" s="25">
         <f t="shared" ref="J33" si="8">J27+1</f>
         <v>6</v>
       </c>
@@ -1932,38 +1962,38 @@
       <c r="L33" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N33" s="23">
+      <c r="N33" s="25">
         <f t="shared" ref="N33" si="9">N27+1</f>
         <v>14</v>
       </c>
       <c r="O33" s="17">
         <v>912</v>
       </c>
-      <c r="P33" s="20" t="s">
+      <c r="P33" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J34" s="24"/>
+      <c r="J34" s="26"/>
       <c r="K34" s="5">
         <v>791.9</v>
       </c>
-      <c r="L34" s="21" t="s">
+      <c r="L34" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="N34" s="24"/>
+      <c r="N34" s="26"/>
       <c r="O34" s="5">
         <v>915</v>
       </c>
-      <c r="P34" s="21"/>
+      <c r="P34" s="23"/>
     </row>
     <row r="35" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J35" s="24"/>
+      <c r="J35" s="26"/>
       <c r="K35" s="5">
         <v>794.9</v>
       </c>
-      <c r="L35" s="21"/>
-      <c r="N35" s="24"/>
+      <c r="L35" s="23"/>
+      <c r="N35" s="26"/>
       <c r="O35" s="5">
         <v>918</v>
       </c>
@@ -1972,14 +2002,14 @@
       </c>
     </row>
     <row r="36" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J36" s="24"/>
+      <c r="J36" s="26"/>
       <c r="K36" s="5">
         <v>797.9</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N36" s="24"/>
+      <c r="N36" s="26"/>
       <c r="O36" s="5">
         <v>920.95</v>
       </c>
@@ -1988,14 +2018,14 @@
       </c>
     </row>
     <row r="37" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J37" s="24"/>
+      <c r="J37" s="26"/>
       <c r="K37" s="5">
         <v>800.7</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N37" s="24"/>
+      <c r="N37" s="26"/>
       <c r="O37" s="5">
         <v>922.9</v>
       </c>
@@ -2004,14 +2034,14 @@
       </c>
     </row>
     <row r="38" spans="10:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J38" s="25"/>
+      <c r="J38" s="27"/>
       <c r="K38" s="6">
         <v>801.8</v>
       </c>
       <c r="L38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N38" s="25"/>
+      <c r="N38" s="27"/>
       <c r="O38" s="6">
         <v>923.75</v>
       </c>
@@ -2020,103 +2050,103 @@
       </c>
     </row>
     <row r="39" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J39" s="27">
+      <c r="J39" s="29">
         <f t="shared" ref="J39" si="10">J33+1</f>
         <v>7</v>
       </c>
-      <c r="K39" s="30">
+      <c r="K39" s="20">
         <v>803.85</v>
       </c>
-      <c r="L39" s="20" t="s">
+      <c r="L39" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N39" s="23">
+      <c r="N39" s="25">
         <f t="shared" ref="N39" si="11">N33+1</f>
         <v>15</v>
       </c>
-      <c r="O39" s="30">
+      <c r="O39" s="20">
         <v>925.8</v>
       </c>
-      <c r="P39" s="20" t="s">
+      <c r="P39" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J40" s="28"/>
-      <c r="K40" s="31">
+      <c r="J40" s="30"/>
+      <c r="K40" s="21">
         <v>806.9</v>
       </c>
-      <c r="L40" s="21"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="31">
+      <c r="L40" s="23"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="21">
         <f>O39+3</f>
         <v>928.8</v>
       </c>
-      <c r="P40" s="21"/>
+      <c r="P40" s="23"/>
     </row>
     <row r="41" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J41" s="28"/>
-      <c r="K41" s="31">
+      <c r="J41" s="30"/>
+      <c r="K41" s="21">
         <v>809.9</v>
       </c>
-      <c r="L41" s="21"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="31">
+      <c r="L41" s="23"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="21">
         <v>931.75</v>
       </c>
-      <c r="P41" s="21"/>
+      <c r="P41" s="23"/>
     </row>
     <row r="42" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J42" s="28"/>
-      <c r="K42" s="31">
+      <c r="J42" s="30"/>
+      <c r="K42" s="21">
         <v>812.9</v>
       </c>
-      <c r="L42" s="21"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="31">
+      <c r="L42" s="23"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="21">
         <f>O41+3</f>
         <v>934.75</v>
       </c>
-      <c r="P42" s="21"/>
+      <c r="P42" s="23"/>
     </row>
     <row r="43" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J43" s="28"/>
-      <c r="K43" s="31">
+      <c r="J43" s="30"/>
+      <c r="K43" s="21">
         <v>815.9</v>
       </c>
-      <c r="L43" s="21"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="31">
+      <c r="L43" s="23"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="21">
         <f>O42+3</f>
         <v>937.75</v>
       </c>
-      <c r="P43" s="21"/>
+      <c r="P43" s="23"/>
     </row>
     <row r="44" spans="10:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="29"/>
-      <c r="K44" s="32">
+      <c r="J44" s="31"/>
+      <c r="K44" s="22">
         <v>818.9</v>
       </c>
-      <c r="L44" s="22"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="32">
+      <c r="L44" s="28"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="22">
         <f>O43+3</f>
         <v>940.75</v>
       </c>
-      <c r="P44" s="22"/>
+      <c r="P44" s="28"/>
     </row>
     <row r="45" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J45" s="23">
+      <c r="J45" s="25">
         <f t="shared" ref="J45" si="12">J39+1</f>
         <v>8</v>
       </c>
       <c r="K45" s="9">
         <v>821.9</v>
       </c>
-      <c r="L45" s="20" t="s">
+      <c r="L45" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="N45" s="23">
+      <c r="N45" s="25">
         <f t="shared" ref="N45" si="13">N39+1</f>
         <v>16</v>
       </c>
@@ -2124,32 +2154,32 @@
         <f>O44+3</f>
         <v>943.75</v>
       </c>
-      <c r="P45" s="20" t="s">
+      <c r="P45" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J46" s="24"/>
+      <c r="J46" s="26"/>
       <c r="K46" s="10">
         <v>824.9</v>
       </c>
-      <c r="L46" s="21"/>
-      <c r="N46" s="24"/>
+      <c r="L46" s="23"/>
+      <c r="N46" s="26"/>
       <c r="O46" s="10">
         <f>O45+3</f>
         <v>946.75</v>
       </c>
-      <c r="P46" s="21"/>
+      <c r="P46" s="23"/>
     </row>
     <row r="47" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J47" s="24"/>
+      <c r="J47" s="26"/>
       <c r="K47" s="14">
         <v>827.85</v>
       </c>
-      <c r="L47" s="21" t="s">
+      <c r="L47" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="N47" s="24"/>
+      <c r="N47" s="26"/>
       <c r="O47" s="10">
         <f t="shared" ref="O47" si="14">O46+3</f>
         <v>949.75</v>
@@ -2159,12 +2189,12 @@
       </c>
     </row>
     <row r="48" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J48" s="24"/>
+      <c r="J48" s="26"/>
       <c r="K48" s="10">
         <v>829.85</v>
       </c>
-      <c r="L48" s="21"/>
-      <c r="N48" s="24"/>
+      <c r="L48" s="23"/>
+      <c r="N48" s="26"/>
       <c r="O48" s="10">
         <v>951.75</v>
       </c>
@@ -2173,14 +2203,14 @@
       </c>
     </row>
     <row r="49" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J49" s="24"/>
+      <c r="J49" s="26"/>
       <c r="K49" s="10">
         <v>831.8</v>
       </c>
       <c r="L49" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N49" s="24"/>
+      <c r="N49" s="26"/>
       <c r="O49" s="10">
         <v>953.45</v>
       </c>
@@ -2189,14 +2219,14 @@
       </c>
     </row>
     <row r="50" spans="10:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="25"/>
+      <c r="J50" s="27"/>
       <c r="K50" s="11" t="s">
         <v>8</v>
       </c>
       <c r="L50" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N50" s="25"/>
+      <c r="N50" s="27"/>
       <c r="O50" s="11" t="s">
         <v>8</v>
       </c>
@@ -2206,6 +2236,39 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P39:P44"/>
+    <mergeCell ref="P45:P46"/>
+    <mergeCell ref="R21:R26"/>
+    <mergeCell ref="P29:P32"/>
+    <mergeCell ref="R3:R8"/>
+    <mergeCell ref="T4:T8"/>
+    <mergeCell ref="R9:R14"/>
+    <mergeCell ref="R15:R20"/>
+    <mergeCell ref="T15:T20"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="P4:P8"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="P15:P20"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="N39:N44"/>
+    <mergeCell ref="N45:N50"/>
+    <mergeCell ref="N9:N14"/>
+    <mergeCell ref="N15:N20"/>
+    <mergeCell ref="N21:N26"/>
+    <mergeCell ref="N3:N8"/>
+    <mergeCell ref="N27:N32"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="L27:L32"/>
+    <mergeCell ref="J33:J38"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="J3:J8"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="L15:L20"/>
+    <mergeCell ref="N33:N38"/>
     <mergeCell ref="L24:L25"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="J15:J20"/>
@@ -2214,41 +2277,8 @@
     <mergeCell ref="L45:L46"/>
     <mergeCell ref="L34:L35"/>
     <mergeCell ref="L47:L48"/>
-    <mergeCell ref="N3:N8"/>
-    <mergeCell ref="N27:N32"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="L27:L32"/>
-    <mergeCell ref="J33:J38"/>
     <mergeCell ref="J39:J44"/>
     <mergeCell ref="L39:L44"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="J3:J8"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="J9:J14"/>
-    <mergeCell ref="L15:L20"/>
-    <mergeCell ref="N33:N38"/>
-    <mergeCell ref="N39:N44"/>
-    <mergeCell ref="N45:N50"/>
-    <mergeCell ref="N9:N14"/>
-    <mergeCell ref="N15:N20"/>
-    <mergeCell ref="N21:N26"/>
-    <mergeCell ref="P4:P8"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="P15:P20"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="R3:R8"/>
-    <mergeCell ref="T4:T8"/>
-    <mergeCell ref="R9:R14"/>
-    <mergeCell ref="R15:R20"/>
-    <mergeCell ref="T15:T20"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P39:P44"/>
-    <mergeCell ref="P45:P46"/>
-    <mergeCell ref="R21:R26"/>
-    <mergeCell ref="P29:P32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>